<commit_message>
Update code :  - the 3 zones are added  - Option to change type of crossroad and number of road for each Update documentation and work diary
</commit_message>
<xml_diff>
--- a/Documentation/FBN_TPI_simulateur_trafic_routier_journal_travail.xlsx
+++ b/Documentation/FBN_TPI_simulateur_trafic_routier_journal_travail.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8730"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -239,6 +239,15 @@
   </si>
   <si>
     <t>Diagramme de flux</t>
+  </si>
+  <si>
+    <t>Mise en place des options - intégration du type de giratoire</t>
+  </si>
+  <si>
+    <t>Mise en place des options - intégration du nombre de routes</t>
+  </si>
+  <si>
+    <t>Mise en place des options - intégration du nombre de véhicules par route</t>
   </si>
 </sst>
 </file>
@@ -752,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,8 +785,8 @@
         <v>4</v>
       </c>
       <c r="B2" s="23">
-        <f>Journal!C46</f>
-        <v>0.28124999999999994</v>
+        <f>Journal!C48</f>
+        <v>0.43749999999999994</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.25">
@@ -785,7 +794,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="24">
-        <f>Journal!C50</f>
+        <f>Journal!C52</f>
         <v>0</v>
       </c>
     </row>
@@ -794,7 +803,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="25">
-        <f>Journal!C54</f>
+        <f>Journal!C56</f>
         <v>0</v>
       </c>
     </row>
@@ -803,7 +812,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="26">
-        <f>Journal!C58</f>
+        <f>Journal!C60</f>
         <v>0</v>
       </c>
     </row>
@@ -813,7 +822,7 @@
       </c>
       <c r="B6" s="27">
         <f>SUM(B1:B5)</f>
-        <v>1.21875</v>
+        <v>1.375</v>
       </c>
     </row>
   </sheetData>
@@ -827,10 +836,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1579,136 +1588,169 @@
       </c>
     </row>
     <row r="44" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="10"/>
-      <c r="E44" s="12"/>
-    </row>
-    <row r="45" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="2"/>
+      <c r="A44" s="4">
+        <v>43600</v>
+      </c>
+      <c r="B44" s="20">
+        <v>3</v>
+      </c>
+      <c r="C44" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>43600</v>
+      </c>
+      <c r="B45" s="20">
+        <v>3</v>
+      </c>
+      <c r="C45" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="46" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="4">
+        <v>43600</v>
+      </c>
+      <c r="B46" s="20">
         <v>3</v>
       </c>
       <c r="C46" s="10">
-        <f>SUM(C36:C45)</f>
-        <v>0.28124999999999994</v>
-      </c>
-      <c r="E46" s="12"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="28" t="s">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="10">
+        <f>SUM(C36:C47)</f>
+        <v>0.43749999999999994</v>
+      </c>
+      <c r="E48" s="12"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="28"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-    </row>
-    <row r="48" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="10"/>
-      <c r="E48" s="12"/>
-    </row>
-    <row r="49" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="2"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
     </row>
     <row r="50" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="C50" s="10"/>
+      <c r="E50" s="12"/>
+    </row>
+    <row r="51" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C50" s="10">
-        <f>SUM(C48:C48)</f>
+      <c r="C52" s="10">
+        <f>SUM(C50:C50)</f>
         <v>0</v>
       </c>
-      <c r="E50" s="12"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
+      <c r="E52" s="12"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="28"/>
-      <c r="F51" s="28"/>
-    </row>
-    <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="10"/>
-      <c r="E52" s="12"/>
-    </row>
-    <row r="53" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="2"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
     </row>
     <row r="54" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="C54" s="10"/>
+      <c r="E54" s="12"/>
+    </row>
+    <row r="55" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C54" s="10">
-        <f>SUM(C52:C52)</f>
+      <c r="C56" s="10">
+        <f>SUM(C54:C54)</f>
         <v>0</v>
       </c>
-      <c r="E54" s="12"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
+      <c r="E56" s="12"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="28"/>
-    </row>
-    <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="10"/>
-      <c r="E56" s="12"/>
-    </row>
-    <row r="57" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="21"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="2"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
     </row>
     <row r="58" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="C58" s="10"/>
+      <c r="E58" s="12"/>
+    </row>
+    <row r="59" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C58" s="10">
-        <f>SUM(C56:C56)</f>
+      <c r="C60" s="10">
+        <f>SUM(C58:C58)</f>
         <v>0</v>
       </c>
-      <c r="E58" s="12"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
+      <c r="E60" s="12"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
@@ -1738,14 +1780,28 @@
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
     </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A57:F57"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A49:F49"/>
+    <mergeCell ref="A53:F53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="92" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Code and Documentation :  - Code : 	- All options works 			- Crossroad integreted
</commit_message>
<xml_diff>
--- a/Documentation/FBN_TPI_simulateur_trafic_routier_journal_travail.xlsx
+++ b/Documentation/FBN_TPI_simulateur_trafic_routier_journal_travail.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -248,6 +248,36 @@
   </si>
   <si>
     <t>Mise en place des options - intégration du nombre de véhicules par route</t>
+  </si>
+  <si>
+    <t>Mise en place des options - suite de l'intégration du nombre de véhicules par route</t>
+  </si>
+  <si>
+    <t>Mise en place des options - Intégration de la vitesse des véhicules</t>
+  </si>
+  <si>
+    <t>Mise en place de la zone de la simulation</t>
+  </si>
+  <si>
+    <t>Mise en place de la zone du résultat de la simulation</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Création du document des résultats et test de l'interface</t>
+  </si>
+  <si>
+    <t>Incorporation du carrefour de priorité de droite</t>
+  </si>
+  <si>
+    <t>Incorporation du carrefour de feux (rouge / vert)</t>
+  </si>
+  <si>
+    <t>Incorporation des giratoires</t>
+  </si>
+  <si>
+    <t>Tests de la séléction des carrefours</t>
   </si>
 </sst>
 </file>
@@ -259,7 +289,7 @@
     <numFmt numFmtId="165" formatCode="hh&quot;h &quot;mm&quot;m &quot;"/>
     <numFmt numFmtId="166" formatCode="[hh]&quot;h &quot;mm&quot;m &quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +300,29 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,7 +378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -386,11 +439,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB1BBCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB1BBCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB1BBCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB1BBCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -473,11 +541,20 @@
     <xf numFmtId="166" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -762,7 +839,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,8 +862,8 @@
         <v>4</v>
       </c>
       <c r="B2" s="23">
-        <f>Journal!C48</f>
-        <v>0.43749999999999994</v>
+        <f>Journal!C57</f>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.25">
@@ -794,7 +871,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="24">
-        <f>Journal!C52</f>
+        <f>Journal!C61</f>
         <v>0</v>
       </c>
     </row>
@@ -803,7 +880,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="25">
-        <f>Journal!C56</f>
+        <f>Journal!C65</f>
         <v>0</v>
       </c>
     </row>
@@ -812,7 +889,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="26">
-        <f>Journal!C60</f>
+        <f>Journal!C69</f>
         <v>0</v>
       </c>
     </row>
@@ -822,7 +899,7 @@
       </c>
       <c r="B6" s="27">
         <f>SUM(B1:B5)</f>
-        <v>1.375</v>
+        <v>1.875</v>
       </c>
     </row>
   </sheetData>
@@ -836,10 +913,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -853,15 +931,15 @@
     <col min="7" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:6" s="28" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -884,14 +962,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:6" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -1442,14 +1520,14 @@
       <c r="E34" s="12"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
     </row>
     <row r="36" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
@@ -1468,340 +1546,512 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+    <row r="37" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
         <v>43599</v>
       </c>
-      <c r="B37" s="20">
+      <c r="B37" s="21">
         <v>2</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="11">
         <v>3.125E-2</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
         <v>43599</v>
       </c>
-      <c r="B38" s="20">
+      <c r="B38" s="21">
         <v>3</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="11">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="13" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
         <v>43599</v>
       </c>
-      <c r="B39" s="20">
+      <c r="B39" s="21">
         <v>3</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="11">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="13" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
         <v>43599</v>
       </c>
-      <c r="B40" s="20">
+      <c r="B40" s="21">
         <v>3</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="11">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="13" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
         <v>43599</v>
       </c>
-      <c r="B41" s="20">
+      <c r="B41" s="21">
         <v>3</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="11">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
         <v>43599</v>
       </c>
-      <c r="B42" s="20">
+      <c r="B42" s="21">
         <v>3</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="11">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="13" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
         <v>43599</v>
       </c>
-      <c r="B43" s="20">
+      <c r="B43" s="21">
         <v>3</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="11">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="13" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
         <v>43600</v>
       </c>
-      <c r="B44" s="20">
+      <c r="B44" s="21">
         <v>3</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="11">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="13" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
         <v>43600</v>
       </c>
-      <c r="B45" s="20">
+      <c r="B45" s="21">
         <v>3</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="11">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E45" s="13" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
         <v>43600</v>
       </c>
-      <c r="B46" s="20">
+      <c r="B46" s="21">
         <v>3</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="11">
         <v>3.125E-2</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="13" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="13"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" s="8" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>43601</v>
+      </c>
+      <c r="B47" s="21">
+        <v>3</v>
+      </c>
+      <c r="C47" s="11">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+    <row r="48" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>43601</v>
+      </c>
+      <c r="B48" s="21">
         <v>3</v>
       </c>
-      <c r="C48" s="10">
-        <f>SUM(C36:C47)</f>
-        <v>0.43749999999999994</v>
-      </c>
-      <c r="E48" s="12"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
+      <c r="C48" s="11">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>43601</v>
+      </c>
+      <c r="B49" s="21">
+        <v>3</v>
+      </c>
+      <c r="C49" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>43601</v>
+      </c>
+      <c r="B50" s="21">
+        <v>3</v>
+      </c>
+      <c r="C50" s="11">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>43601</v>
+      </c>
+      <c r="B51" s="21">
+        <v>3</v>
+      </c>
+      <c r="C51" s="11">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>43602</v>
+      </c>
+      <c r="B52" s="21">
+        <v>4</v>
+      </c>
+      <c r="C52" s="11">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <v>43602</v>
+      </c>
+      <c r="B53" s="21">
+        <v>4</v>
+      </c>
+      <c r="C53" s="11">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E53" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <v>43602</v>
+      </c>
+      <c r="B54" s="21">
+        <v>4</v>
+      </c>
+      <c r="C54" s="11">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E54" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
+        <v>43602</v>
+      </c>
+      <c r="B55" s="21">
+        <v>4</v>
+      </c>
+      <c r="C55" s="11">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="10">
+        <f>SUM(C36:C56)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="E57" s="12"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="28"/>
-    </row>
-    <row r="50" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="10"/>
-      <c r="E50" s="12"/>
-    </row>
-    <row r="51" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+      <c r="B58" s="29"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
+    </row>
+    <row r="59" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="10"/>
+      <c r="E59" s="12"/>
+    </row>
+    <row r="60" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="10">
-        <f>SUM(C50:C50)</f>
+      <c r="C61" s="10">
+        <f>SUM(C59:C59)</f>
         <v>0</v>
       </c>
-      <c r="E52" s="12"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="28" t="s">
+      <c r="E61" s="12"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-    </row>
-    <row r="54" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="10"/>
-      <c r="E54" s="12"/>
-    </row>
-    <row r="55" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="21"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="29"/>
+      <c r="F62" s="29"/>
+    </row>
+    <row r="63" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C63" s="10"/>
+      <c r="E63" s="12"/>
+    </row>
+    <row r="64" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C56" s="10">
-        <f>SUM(C54:C54)</f>
+      <c r="C65" s="10">
+        <f>SUM(C63:C63)</f>
         <v>0</v>
       </c>
-      <c r="E56" s="12"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="28" t="s">
+      <c r="E65" s="12"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-    </row>
-    <row r="58" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="10"/>
-      <c r="E58" s="12"/>
-    </row>
-    <row r="59" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="21"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
+    </row>
+    <row r="67" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="10"/>
+      <c r="E67" s="12"/>
+    </row>
+    <row r="68" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="10">
-        <f>SUM(C58:C58)</f>
+      <c r="C69" s="10">
+        <f>SUM(C67:C67)</f>
         <v>0</v>
       </c>
-      <c r="E60" s="12"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="6"/>
-      <c r="F62" s="6"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="6"/>
-      <c r="F65" s="6"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="6"/>
+      <c r="E69" s="12"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="5"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A66:F66"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A49:F49"/>
-    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A62:F62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="92" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update code and documentation :  - Change crossroad to object function  - Add not working code to place vehicle  - Update work diary  - Update planification
</commit_message>
<xml_diff>
--- a/Documentation/FBN_TPI_simulateur_trafic_routier_journal_travail.xlsx
+++ b/Documentation/FBN_TPI_simulateur_trafic_routier_journal_travail.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -278,6 +278,36 @@
   </si>
   <si>
     <t>Tests de la séléction des carrefours</t>
+  </si>
+  <si>
+    <t>Suite des tests de la séléction des carrefours</t>
+  </si>
+  <si>
+    <t>Entretien avec le 2ème expert, M. Yves Bertino</t>
+  </si>
+  <si>
+    <t>Définition des règles de conduite</t>
+  </si>
+  <si>
+    <t>Implémentation des images des véhicules</t>
+  </si>
+  <si>
+    <t>Impélémentation de la génération des véhicules - Définition de l'objet véhicule</t>
+  </si>
+  <si>
+    <t>Impélémentation de la génération des véhicules - Appel de l'objet et création des listes de véhicules</t>
+  </si>
+  <si>
+    <t>Implémentation du placement des véhicules - Création de la fonction de détéction du point de départ</t>
+  </si>
+  <si>
+    <t>Implémentation du placement des véhicules - Suite de la création de la fonction précédente</t>
+  </si>
+  <si>
+    <t>Implémentation du placement des véhicules - Détermintation du décalge à chaque route suplémentaire</t>
+  </si>
+  <si>
+    <t>Modification des carrefours, passage à un objet pour plus de facilité</t>
   </si>
 </sst>
 </file>
@@ -544,17 +574,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -838,7 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -871,8 +901,8 @@
         <v>5</v>
       </c>
       <c r="B3" s="24">
-        <f>Journal!C61</f>
-        <v>0</v>
+        <f>Journal!C70</f>
+        <v>0.43750000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.25">
@@ -880,7 +910,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="25">
-        <f>Journal!C65</f>
+        <f>Journal!C74</f>
         <v>0</v>
       </c>
     </row>
@@ -889,7 +919,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="26">
-        <f>Journal!C69</f>
+        <f>Journal!C78</f>
         <v>0</v>
       </c>
     </row>
@@ -899,7 +929,7 @@
       </c>
       <c r="B6" s="27">
         <f>SUM(B1:B5)</f>
-        <v>1.875</v>
+        <v>2.3125</v>
       </c>
     </row>
   </sheetData>
@@ -913,11 +943,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -932,14 +962,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="28" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -962,14 +992,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -1520,14 +1550,14 @@
       <c r="E34" s="12"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
     </row>
     <row r="36" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
@@ -1829,7 +1859,7 @@
       <c r="D52" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E52" s="31" t="s">
+      <c r="E52" s="29" t="s">
         <v>78</v>
       </c>
       <c r="F52" s="2"/>
@@ -1847,7 +1877,7 @@
       <c r="D53" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E53" s="31" t="s">
+      <c r="E53" s="29" t="s">
         <v>79</v>
       </c>
       <c r="F53" s="2"/>
@@ -1865,7 +1895,7 @@
       <c r="D54" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E54" s="31" t="s">
+      <c r="E54" s="29" t="s">
         <v>80</v>
       </c>
       <c r="F54" s="2"/>
@@ -1881,9 +1911,9 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E55" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="E55" s="30" t="s">
         <v>81</v>
       </c>
       <c r="F55" s="2"/>
@@ -1907,151 +1937,324 @@
       <c r="E57" s="12"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="29" t="s">
+      <c r="A58" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B58" s="29"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="31"/>
     </row>
     <row r="59" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="10"/>
-      <c r="E59" s="12"/>
+      <c r="A59" s="4">
+        <v>43606</v>
+      </c>
+      <c r="B59" s="20">
+        <v>4</v>
+      </c>
+      <c r="C59" s="10">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="60" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="13"/>
+      <c r="A60" s="7">
+        <v>43606</v>
+      </c>
+      <c r="B60" s="21">
+        <v>5</v>
+      </c>
+      <c r="C60" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>83</v>
+      </c>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
+        <v>43606</v>
+      </c>
+      <c r="B61" s="21">
+        <v>5</v>
+      </c>
+      <c r="C61" s="11">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
+        <v>43606</v>
+      </c>
+      <c r="B62" s="21">
+        <v>5</v>
+      </c>
+      <c r="C62" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" s="8" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
+        <v>43606</v>
+      </c>
+      <c r="B63" s="21">
+        <v>5</v>
+      </c>
+      <c r="C63" s="11">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" s="8" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
+        <v>43606</v>
+      </c>
+      <c r="B64" s="21">
+        <v>5</v>
+      </c>
+      <c r="C64" s="11">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D64" s="3"/>
+      <c r="E64" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" s="8" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7">
+        <v>43606</v>
+      </c>
+      <c r="B65" s="21">
+        <v>5</v>
+      </c>
+      <c r="C65" s="11">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="7">
+        <v>43607</v>
+      </c>
+      <c r="B66" s="21">
+        <v>5</v>
+      </c>
+      <c r="C66" s="11">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E66" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="7">
+        <v>43607</v>
+      </c>
+      <c r="B67" s="21">
+        <v>5</v>
+      </c>
+      <c r="C67" s="11">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7">
+        <v>43607</v>
+      </c>
+      <c r="B68" s="21">
+        <v>5</v>
+      </c>
+      <c r="C68" s="11">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E68" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="7"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="10">
-        <f>SUM(C59:C59)</f>
+      <c r="C70" s="10">
+        <f>SUM(C59:C69)</f>
+        <v>0.43750000000000006</v>
+      </c>
+      <c r="E70" s="12"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B71" s="31"/>
+      <c r="C71" s="31"/>
+      <c r="D71" s="31"/>
+      <c r="E71" s="31"/>
+      <c r="F71" s="31"/>
+    </row>
+    <row r="72" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="10"/>
+      <c r="E72" s="12"/>
+    </row>
+    <row r="73" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="7"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="10">
+        <f>SUM(C72:C72)</f>
         <v>0</v>
       </c>
-      <c r="E61" s="12"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B62" s="29"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="29"/>
-      <c r="E62" s="29"/>
-      <c r="F62" s="29"/>
-    </row>
-    <row r="63" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="10"/>
-      <c r="E63" s="12"/>
-    </row>
-    <row r="64" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+      <c r="E74" s="12"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B75" s="31"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="31"/>
+      <c r="F75" s="31"/>
+    </row>
+    <row r="76" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="10"/>
+      <c r="E76" s="12"/>
+    </row>
+    <row r="77" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="7"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="10">
-        <f>SUM(C63:C63)</f>
+      <c r="C78" s="10">
+        <f>SUM(C76:C76)</f>
         <v>0</v>
       </c>
-      <c r="E65" s="12"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="B66" s="29"/>
-      <c r="C66" s="29"/>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29"/>
-      <c r="F66" s="29"/>
-    </row>
-    <row r="67" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="10"/>
-      <c r="E67" s="12"/>
-    </row>
-    <row r="68" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
-      <c r="B68" s="21"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="2"/>
-    </row>
-    <row r="69" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C69" s="10">
-        <f>SUM(C67:C67)</f>
-        <v>0</v>
-      </c>
-      <c r="E69" s="12"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
+      <c r="E78" s="12"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="5"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="5"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="5"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="5"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="A75:F75"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A35:F35"/>
     <mergeCell ref="A58:F58"/>
-    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A71:F71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="92" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update documentation and work diary :  - many small elements are updated : 	- UML 	- Test strategy 	- List of documents 	- Others
</commit_message>
<xml_diff>
--- a/Documentation/FBN_TPI_simulateur_trafic_routier_journal_travail.xlsx
+++ b/Documentation/FBN_TPI_simulateur_trafic_routier_journal_travail.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="97">
   <si>
     <t>Date</t>
   </si>
@@ -214,9 +214,6 @@
     <t>Sprint</t>
   </si>
   <si>
-    <t>Analyse</t>
-  </si>
-  <si>
     <t>Conception</t>
   </si>
   <si>
@@ -308,6 +305,24 @@
   </si>
   <si>
     <t>Modification des carrefours, passage à un objet pour plus de facilité</t>
+  </si>
+  <si>
+    <t>Suite et fin de l'implémentation du placement des véhicules</t>
+  </si>
+  <si>
+    <t>Tests de la partie véhicule de la génération de la simulation</t>
+  </si>
+  <si>
+    <t>Ajout des résultats de la simulation dans le diagramme des cas d'utilisations</t>
+  </si>
+  <si>
+    <t>Définition des uses cases du résultat de la simulation - priorités de droite</t>
+  </si>
+  <si>
+    <t>Définition des uses cases du résultat de la simulation - feux</t>
+  </si>
+  <si>
+    <t>Définition des uses cases du résultat de la simulation - giratoires</t>
   </si>
 </sst>
 </file>
@@ -901,8 +916,8 @@
         <v>5</v>
       </c>
       <c r="B3" s="24">
-        <f>Journal!C70</f>
-        <v>0.43750000000000006</v>
+        <f>Journal!C77</f>
+        <v>0.71875000000000011</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.25">
@@ -910,7 +925,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="25">
-        <f>Journal!C74</f>
+        <f>Journal!C81</f>
         <v>0</v>
       </c>
     </row>
@@ -919,7 +934,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="26">
-        <f>Journal!C78</f>
+        <f>Journal!C85</f>
         <v>0</v>
       </c>
     </row>
@@ -929,7 +944,7 @@
       </c>
       <c r="B6" s="27">
         <f>SUM(B1:B5)</f>
-        <v>2.3125</v>
+        <v>2.59375</v>
       </c>
     </row>
   </sheetData>
@@ -943,11 +958,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1605,10 +1620,10 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F38" s="2"/>
     </row>
@@ -1623,10 +1638,10 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="D39" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="F39" s="2"/>
     </row>
@@ -1641,10 +1656,10 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F40" s="2"/>
     </row>
@@ -1659,10 +1674,10 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F41" s="2"/>
     </row>
@@ -1677,10 +1692,10 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D42" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>65</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>66</v>
       </c>
       <c r="F42" s="2"/>
     </row>
@@ -1695,10 +1710,10 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F43" s="2"/>
     </row>
@@ -1713,10 +1728,10 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F44" s="2"/>
     </row>
@@ -1731,10 +1746,10 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F45" s="2"/>
     </row>
@@ -1749,10 +1764,10 @@
         <v>3.125E-2</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F46" s="2"/>
     </row>
@@ -1767,10 +1782,10 @@
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F47" s="2"/>
     </row>
@@ -1785,10 +1800,10 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F48" s="2"/>
     </row>
@@ -1803,10 +1818,10 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F49" s="2"/>
     </row>
@@ -1821,10 +1836,10 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F50" s="2"/>
     </row>
@@ -1839,10 +1854,10 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D51" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E51" s="13" t="s">
         <v>76</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>77</v>
       </c>
       <c r="F51" s="2"/>
     </row>
@@ -1857,10 +1872,10 @@
         <v>6.25E-2</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F52" s="2"/>
     </row>
@@ -1875,10 +1890,10 @@
         <v>6.25E-2</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E53" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F53" s="2"/>
     </row>
@@ -1893,10 +1908,10 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F54" s="2"/>
     </row>
@@ -1911,10 +1926,10 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E55" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F55" s="2"/>
     </row>
@@ -1957,10 +1972,10 @@
         <v>3.125E-2</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1977,7 +1992,7 @@
         <v>22</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F60" s="2"/>
     </row>
@@ -1995,7 +2010,7 @@
         <v>23</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F61" s="2"/>
     </row>
@@ -2010,10 +2025,10 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F62" s="2"/>
     </row>
@@ -2028,10 +2043,10 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F63" s="2"/>
     </row>
@@ -2047,7 +2062,7 @@
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F64" s="2"/>
     </row>
@@ -2062,10 +2077,10 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F65" s="2"/>
     </row>
@@ -2080,10 +2095,10 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E66" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F66" s="2"/>
     </row>
@@ -2098,10 +2113,10 @@
         <v>7.2916666666666671E-2</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E67" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F67" s="2"/>
     </row>
@@ -2116,145 +2131,269 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E68" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="7">
+        <v>43608</v>
+      </c>
+      <c r="B69" s="21">
+        <v>5</v>
+      </c>
+      <c r="C69" s="11">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E69" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="F68" s="2"/>
-    </row>
-    <row r="69" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="7"/>
-      <c r="B69" s="21"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="13"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
+    <row r="70" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="7">
+        <v>43608</v>
+      </c>
+      <c r="B70" s="21">
+        <v>5</v>
+      </c>
+      <c r="C70" s="11">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E70" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
+        <v>43608</v>
+      </c>
+      <c r="B71" s="21">
+        <v>6</v>
+      </c>
+      <c r="C71" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="7">
+        <v>43608</v>
+      </c>
+      <c r="B72" s="21">
+        <v>6</v>
+      </c>
+      <c r="C72" s="11">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E72" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="7">
+        <v>43608</v>
+      </c>
+      <c r="B73" s="21">
+        <v>6</v>
+      </c>
+      <c r="C73" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E73" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="7">
+        <v>43608</v>
+      </c>
+      <c r="B74" s="21">
+        <v>6</v>
+      </c>
+      <c r="C74" s="11">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E74" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="7">
+        <v>43608</v>
+      </c>
+      <c r="B75" s="21">
+        <v>6</v>
+      </c>
+      <c r="C75" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E75" s="29"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="7"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C70" s="10">
-        <f>SUM(C59:C69)</f>
-        <v>0.43750000000000006</v>
-      </c>
-      <c r="E70" s="12"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="31" t="s">
+      <c r="C77" s="10">
+        <f>SUM(C59:C76)</f>
+        <v>0.71875000000000011</v>
+      </c>
+      <c r="E77" s="12"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B71" s="31"/>
-      <c r="C71" s="31"/>
-      <c r="D71" s="31"/>
-      <c r="E71" s="31"/>
-      <c r="F71" s="31"/>
-    </row>
-    <row r="72" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C72" s="10"/>
-      <c r="E72" s="12"/>
-    </row>
-    <row r="73" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
-      <c r="B73" s="21"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="2"/>
-    </row>
-    <row r="74" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+      <c r="B78" s="31"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="31"/>
+      <c r="E78" s="31"/>
+      <c r="F78" s="31"/>
+    </row>
+    <row r="79" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="10"/>
+      <c r="E79" s="12"/>
+    </row>
+    <row r="80" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="7"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C74" s="10">
-        <f>SUM(C72:C72)</f>
+      <c r="C81" s="10">
+        <f>SUM(C79:C79)</f>
         <v>0</v>
       </c>
-      <c r="E74" s="12"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="31" t="s">
+      <c r="E81" s="12"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B75" s="31"/>
-      <c r="C75" s="31"/>
-      <c r="D75" s="31"/>
-      <c r="E75" s="31"/>
-      <c r="F75" s="31"/>
-    </row>
-    <row r="76" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C76" s="10"/>
-      <c r="E76" s="12"/>
-    </row>
-    <row r="77" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="7"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="2"/>
-    </row>
-    <row r="78" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+      <c r="B82" s="31"/>
+      <c r="C82" s="31"/>
+      <c r="D82" s="31"/>
+      <c r="E82" s="31"/>
+      <c r="F82" s="31"/>
+    </row>
+    <row r="83" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C83" s="10"/>
+      <c r="E83" s="12"/>
+    </row>
+    <row r="84" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="7"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C78" s="10">
-        <f>SUM(C76:C76)</f>
+      <c r="C85" s="10">
+        <f>SUM(C83:C83)</f>
         <v>0</v>
       </c>
-      <c r="E78" s="12"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="6"/>
-      <c r="F82" s="6"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="6"/>
-      <c r="F83" s="6"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="6"/>
-      <c r="F84" s="6"/>
+      <c r="E85" s="12"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="5"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="5"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="5"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="A82:F82"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A35:F35"/>
     <mergeCell ref="A58:F58"/>
-    <mergeCell ref="A71:F71"/>
+    <mergeCell ref="A78:F78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="92" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update code and documentation :  - Code : 	- Add function to run simulation 	- Add priority parameter in vehicle object 	- Add begin of result simulation for right priority  - Documentation : 	- Update last uses case 	- Update test dosumentation 	- Update work diary
</commit_message>
<xml_diff>
--- a/Documentation/FBN_TPI_simulateur_trafic_routier_journal_travail.xlsx
+++ b/Documentation/FBN_TPI_simulateur_trafic_routier_journal_travail.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
   <si>
     <t>Date</t>
   </si>
@@ -323,6 +323,18 @@
   </si>
   <si>
     <t>Définition des uses cases du résultat de la simulation - giratoires</t>
+  </si>
+  <si>
+    <t>Création de la fonction du résultat de la simulation</t>
+  </si>
+  <si>
+    <t>Suite de la création de la fonction du résultat de la simulation</t>
+  </si>
+  <si>
+    <t>Implémentation des rêgles de conduites pour les priorités de droite</t>
+  </si>
+  <si>
+    <t>Mise en place de l'ecriture des résultats pour les priorités de droite</t>
   </si>
 </sst>
 </file>
@@ -916,8 +928,8 @@
         <v>5</v>
       </c>
       <c r="B3" s="24">
-        <f>Journal!C77</f>
-        <v>0.71875000000000011</v>
+        <f>Journal!C80</f>
+        <v>0.93750000000000011</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.25">
@@ -925,7 +937,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="25">
-        <f>Journal!C81</f>
+        <f>Journal!C84</f>
         <v>0</v>
       </c>
     </row>
@@ -934,7 +946,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="26">
-        <f>Journal!C85</f>
+        <f>Journal!C88</f>
         <v>0</v>
       </c>
     </row>
@@ -944,7 +956,7 @@
       </c>
       <c r="B6" s="27">
         <f>SUM(B1:B5)</f>
-        <v>2.59375</v>
+        <v>2.8125</v>
       </c>
     </row>
   </sheetData>
@@ -958,11 +970,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <pane ySplit="2" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1221,7 +1233,7 @@
         <v>43593</v>
       </c>
       <c r="B15" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="11">
         <v>2.0833333333333332E-2</v>
@@ -1241,7 +1253,7 @@
         <v>43593</v>
       </c>
       <c r="B16" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="11">
         <v>2.0833333333333332E-2</v>
@@ -1259,7 +1271,7 @@
         <v>43593</v>
       </c>
       <c r="B17" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" s="11">
         <v>3.125E-2</v>
@@ -1277,7 +1289,7 @@
         <v>43593</v>
       </c>
       <c r="B18" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" s="11">
         <v>5.2083333333333336E-2</v>
@@ -1295,7 +1307,7 @@
         <v>43594</v>
       </c>
       <c r="B19" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" s="11">
         <v>2.0833333333333332E-2</v>
@@ -1315,7 +1327,7 @@
         <v>43594</v>
       </c>
       <c r="B20" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="11">
         <v>2.0833333333333332E-2</v>
@@ -1333,7 +1345,7 @@
         <v>43594</v>
       </c>
       <c r="B21" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" s="11">
         <v>1.0416666666666666E-2</v>
@@ -1353,7 +1365,7 @@
         <v>43594</v>
       </c>
       <c r="B22" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22" s="11">
         <v>2.0833333333333332E-2</v>
@@ -1371,7 +1383,7 @@
         <v>43594</v>
       </c>
       <c r="B23" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23" s="11">
         <v>7.2916666666666671E-2</v>
@@ -1389,7 +1401,7 @@
         <v>43594</v>
       </c>
       <c r="B24" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C24" s="11">
         <v>8.3333333333333329E-2</v>
@@ -1407,7 +1419,7 @@
         <v>43594</v>
       </c>
       <c r="B25" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" s="11">
         <v>5.2083333333333336E-2</v>
@@ -1425,7 +1437,7 @@
         <v>43595</v>
       </c>
       <c r="B26" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26" s="11">
         <v>3.125E-2</v>
@@ -1443,7 +1455,7 @@
         <v>43595</v>
       </c>
       <c r="B27" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" s="11">
         <v>2.0833333333333332E-2</v>
@@ -1461,7 +1473,7 @@
         <v>43595</v>
       </c>
       <c r="B28" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28" s="11">
         <v>4.1666666666666664E-2</v>
@@ -1479,7 +1491,7 @@
         <v>43595</v>
       </c>
       <c r="B29" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29" s="11">
         <v>2.0833333333333332E-2</v>
@@ -1497,7 +1509,7 @@
         <v>43595</v>
       </c>
       <c r="B30" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30" s="11">
         <v>6.25E-2</v>
@@ -1515,7 +1527,7 @@
         <v>43595</v>
       </c>
       <c r="B31" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31" s="11">
         <v>3.125E-2</v>
@@ -1533,7 +1545,7 @@
         <v>43595</v>
       </c>
       <c r="B32" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C32" s="11">
         <v>1.0416666666666666E-2</v>
@@ -1579,7 +1591,7 @@
         <v>43599</v>
       </c>
       <c r="B36" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C36" s="10">
         <v>2.0833333333333332E-2</v>
@@ -1596,7 +1608,7 @@
         <v>43599</v>
       </c>
       <c r="B37" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C37" s="11">
         <v>3.125E-2</v>
@@ -1614,7 +1626,7 @@
         <v>43599</v>
       </c>
       <c r="B38" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C38" s="11">
         <v>8.3333333333333329E-2</v>
@@ -1632,7 +1644,7 @@
         <v>43599</v>
       </c>
       <c r="B39" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C39" s="11">
         <v>1.0416666666666666E-2</v>
@@ -1650,7 +1662,7 @@
         <v>43599</v>
       </c>
       <c r="B40" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C40" s="11">
         <v>1.0416666666666666E-2</v>
@@ -1668,7 +1680,7 @@
         <v>43599</v>
       </c>
       <c r="B41" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C41" s="11">
         <v>2.0833333333333332E-2</v>
@@ -1686,7 +1698,7 @@
         <v>43599</v>
       </c>
       <c r="B42" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C42" s="11">
         <v>8.3333333333333329E-2</v>
@@ -1704,7 +1716,7 @@
         <v>43599</v>
       </c>
       <c r="B43" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C43" s="11">
         <v>2.0833333333333332E-2</v>
@@ -1722,7 +1734,7 @@
         <v>43600</v>
       </c>
       <c r="B44" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C44" s="11">
         <v>4.1666666666666664E-2</v>
@@ -1740,7 +1752,7 @@
         <v>43600</v>
       </c>
       <c r="B45" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C45" s="11">
         <v>8.3333333333333329E-2</v>
@@ -1758,7 +1770,7 @@
         <v>43600</v>
       </c>
       <c r="B46" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C46" s="11">
         <v>3.125E-2</v>
@@ -1776,7 +1788,7 @@
         <v>43601</v>
       </c>
       <c r="B47" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C47" s="11">
         <v>5.2083333333333336E-2</v>
@@ -1794,7 +1806,7 @@
         <v>43601</v>
       </c>
       <c r="B48" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C48" s="11">
         <v>4.1666666666666664E-2</v>
@@ -1812,7 +1824,7 @@
         <v>43601</v>
       </c>
       <c r="B49" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C49" s="11">
         <v>2.0833333333333332E-2</v>
@@ -1830,7 +1842,7 @@
         <v>43601</v>
       </c>
       <c r="B50" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C50" s="11">
         <v>8.3333333333333329E-2</v>
@@ -1848,7 +1860,7 @@
         <v>43601</v>
       </c>
       <c r="B51" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C51" s="11">
         <v>8.3333333333333329E-2</v>
@@ -1866,7 +1878,7 @@
         <v>43602</v>
       </c>
       <c r="B52" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C52" s="11">
         <v>6.25E-2</v>
@@ -1884,7 +1896,7 @@
         <v>43602</v>
       </c>
       <c r="B53" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C53" s="11">
         <v>6.25E-2</v>
@@ -1902,7 +1914,7 @@
         <v>43602</v>
       </c>
       <c r="B54" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C54" s="11">
         <v>8.3333333333333329E-2</v>
@@ -1920,7 +1932,7 @@
         <v>43602</v>
       </c>
       <c r="B55" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C55" s="11">
         <v>1.0416666666666666E-2</v>
@@ -1966,7 +1978,7 @@
         <v>43606</v>
       </c>
       <c r="B59" s="20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C59" s="10">
         <v>3.125E-2</v>
@@ -1983,7 +1995,7 @@
         <v>43606</v>
       </c>
       <c r="B60" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C60" s="11">
         <v>2.0833333333333332E-2</v>
@@ -2001,7 +2013,7 @@
         <v>43606</v>
       </c>
       <c r="B61" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C61" s="11">
         <v>4.1666666666666664E-2</v>
@@ -2019,7 +2031,7 @@
         <v>43606</v>
       </c>
       <c r="B62" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C62" s="11">
         <v>2.0833333333333332E-2</v>
@@ -2037,7 +2049,7 @@
         <v>43606</v>
       </c>
       <c r="B63" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C63" s="11">
         <v>8.3333333333333329E-2</v>
@@ -2055,7 +2067,7 @@
         <v>43606</v>
       </c>
       <c r="B64" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C64" s="11">
         <v>4.1666666666666664E-2</v>
@@ -2071,7 +2083,7 @@
         <v>43606</v>
       </c>
       <c r="B65" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C65" s="11">
         <v>4.1666666666666664E-2</v>
@@ -2089,7 +2101,7 @@
         <v>43607</v>
       </c>
       <c r="B66" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C66" s="11">
         <v>4.1666666666666664E-2</v>
@@ -2107,7 +2119,7 @@
         <v>43607</v>
       </c>
       <c r="B67" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C67" s="11">
         <v>7.2916666666666671E-2</v>
@@ -2125,7 +2137,7 @@
         <v>43607</v>
       </c>
       <c r="B68" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C68" s="11">
         <v>4.1666666666666664E-2</v>
@@ -2143,7 +2155,7 @@
         <v>43608</v>
       </c>
       <c r="B69" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C69" s="11">
         <v>5.2083333333333336E-2</v>
@@ -2161,7 +2173,7 @@
         <v>43608</v>
       </c>
       <c r="B70" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C70" s="11">
         <v>4.1666666666666664E-2</v>
@@ -2179,7 +2191,7 @@
         <v>43608</v>
       </c>
       <c r="B71" s="21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C71" s="11">
         <v>2.0833333333333332E-2</v>
@@ -2197,7 +2209,7 @@
         <v>43608</v>
       </c>
       <c r="B72" s="21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C72" s="11">
         <v>8.3333333333333329E-2</v>
@@ -2215,7 +2227,7 @@
         <v>43608</v>
       </c>
       <c r="B73" s="21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C73" s="11">
         <v>2.0833333333333332E-2</v>
@@ -2233,7 +2245,7 @@
         <v>43608</v>
       </c>
       <c r="B74" s="21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C74" s="11">
         <v>4.1666666666666664E-2</v>
@@ -2251,7 +2263,7 @@
         <v>43608</v>
       </c>
       <c r="B75" s="21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C75" s="11">
         <v>2.0833333333333332E-2</v>
@@ -2259,111 +2271,146 @@
       <c r="D75" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E75" s="29"/>
+      <c r="E75" s="29" t="s">
+        <v>97</v>
+      </c>
       <c r="F75" s="2"/>
     </row>
     <row r="76" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="7"/>
-      <c r="B76" s="21"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="13"/>
+      <c r="A76" s="7">
+        <v>43609</v>
+      </c>
+      <c r="B76" s="21">
+        <v>7</v>
+      </c>
+      <c r="C76" s="11">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>98</v>
+      </c>
       <c r="F76" s="2"/>
     </row>
-    <row r="77" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+    <row r="77" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="7">
+        <v>43609</v>
+      </c>
+      <c r="B77" s="21">
+        <v>7</v>
+      </c>
+      <c r="C77" s="11">
+        <v>9.375E-2</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="7">
+        <v>43609</v>
+      </c>
+      <c r="B78" s="21">
+        <v>7</v>
+      </c>
+      <c r="C78" s="11">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E78" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="7"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="10">
-        <f>SUM(C59:C76)</f>
-        <v>0.71875000000000011</v>
-      </c>
-      <c r="E77" s="12"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="31" t="s">
+      <c r="C80" s="10">
+        <f>SUM(C59:C79)</f>
+        <v>0.93750000000000011</v>
+      </c>
+      <c r="E80" s="12"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B78" s="31"/>
-      <c r="C78" s="31"/>
-      <c r="D78" s="31"/>
-      <c r="E78" s="31"/>
-      <c r="F78" s="31"/>
-    </row>
-    <row r="79" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="10"/>
-      <c r="E79" s="12"/>
-    </row>
-    <row r="80" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="7"/>
-      <c r="B80" s="21"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="2"/>
-    </row>
-    <row r="81" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+      <c r="B81" s="31"/>
+      <c r="C81" s="31"/>
+      <c r="D81" s="31"/>
+      <c r="E81" s="31"/>
+      <c r="F81" s="31"/>
+    </row>
+    <row r="82" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C82" s="10"/>
+      <c r="E82" s="12"/>
+    </row>
+    <row r="83" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="7"/>
+      <c r="B83" s="21"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C81" s="10">
-        <f>SUM(C79:C79)</f>
+      <c r="C84" s="10">
+        <f>SUM(C82:C82)</f>
         <v>0</v>
       </c>
-      <c r="E81" s="12"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="31" t="s">
+      <c r="E84" s="12"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B82" s="31"/>
-      <c r="C82" s="31"/>
-      <c r="D82" s="31"/>
-      <c r="E82" s="31"/>
-      <c r="F82" s="31"/>
-    </row>
-    <row r="83" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C83" s="10"/>
-      <c r="E83" s="12"/>
-    </row>
-    <row r="84" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="7"/>
-      <c r="B84" s="21"/>
-      <c r="C84" s="11"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="2"/>
-    </row>
-    <row r="85" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
+      <c r="B85" s="31"/>
+      <c r="C85" s="31"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="31"/>
+    </row>
+    <row r="86" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C86" s="10"/>
+      <c r="E86" s="12"/>
+    </row>
+    <row r="87" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="7"/>
+      <c r="B87" s="21"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C85" s="10">
-        <f>SUM(C83:C83)</f>
+      <c r="C88" s="10">
+        <f>SUM(C86:C86)</f>
         <v>0</v>
       </c>
-      <c r="E85" s="12"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="6"/>
-      <c r="F86" s="6"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="6"/>
-      <c r="F87" s="6"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="6"/>
-      <c r="F88" s="6"/>
+      <c r="E88" s="12"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
@@ -2386,14 +2433,35 @@
       <c r="E91" s="6"/>
       <c r="F91" s="6"/>
     </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="5"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="5"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="5"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A85:F85"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A35:F35"/>
     <mergeCell ref="A58:F58"/>
-    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A81:F81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="92" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update code and documentation :  - Add giratory result and end of trafic light result  - Update test documentation
</commit_message>
<xml_diff>
--- a/Documentation/FBN_TPI_simulateur_trafic_routier_journal_travail.xlsx
+++ b/Documentation/FBN_TPI_simulateur_trafic_routier_journal_travail.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
   <si>
     <t>Date</t>
   </si>
@@ -335,6 +335,30 @@
   </si>
   <si>
     <t>Mise en place de l'ecriture des résultats pour les priorités de droite</t>
+  </si>
+  <si>
+    <t>Suite et fin de l'écriture des résultats pour les priorités de droite</t>
+  </si>
+  <si>
+    <t>Suite de la création de la fonction de la simulation - partie feux vert / rouge</t>
+  </si>
+  <si>
+    <t>Implémentation des rêgles de conduites pour les feux (rouge / vert)</t>
+  </si>
+  <si>
+    <t>Suite de la création de la fonction de la simulation - giratoire</t>
+  </si>
+  <si>
+    <t>Implémentation des rêgles de conduites pour les giratoires</t>
+  </si>
+  <si>
+    <t>Suite et fin de l'implémentation des rêgles de conduite pour les giratoires</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Tests du resultat de la simulation</t>
   </si>
 </sst>
 </file>
@@ -896,7 +920,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,8 +961,8 @@
         <v>6</v>
       </c>
       <c r="B4" s="25">
-        <f>Journal!C84</f>
-        <v>0</v>
+        <f>Journal!C90</f>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="21" x14ac:dyDescent="0.25">
@@ -946,7 +970,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="26">
-        <f>Journal!C88</f>
+        <f>Journal!C94</f>
         <v>0</v>
       </c>
     </row>
@@ -956,7 +980,7 @@
       </c>
       <c r="B6" s="27">
         <f>SUM(B1:B5)</f>
-        <v>2.8125</v>
+        <v>3.25</v>
       </c>
     </row>
   </sheetData>
@@ -970,11 +994,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E79" sqref="E79"/>
+      <pane ySplit="2" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2096,7 +2120,7 @@
       </c>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" s="8" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>43607</v>
       </c>
@@ -2109,12 +2133,12 @@
       <c r="D66" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E66" s="29" t="s">
+      <c r="E66" s="13" t="s">
         <v>88</v>
       </c>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" s="8" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>43607</v>
       </c>
@@ -2127,7 +2151,7 @@
       <c r="D67" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E67" s="29" t="s">
+      <c r="E67" s="13" t="s">
         <v>89</v>
       </c>
       <c r="F67" s="2"/>
@@ -2145,7 +2169,7 @@
       <c r="D68" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E68" s="30" t="s">
+      <c r="E68" s="13" t="s">
         <v>90</v>
       </c>
       <c r="F68" s="2"/>
@@ -2163,7 +2187,7 @@
       <c r="D69" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E69" s="30" t="s">
+      <c r="E69" s="13" t="s">
         <v>91</v>
       </c>
       <c r="F69" s="2"/>
@@ -2181,7 +2205,7 @@
       <c r="D70" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E70" s="30" t="s">
+      <c r="E70" s="13" t="s">
         <v>92</v>
       </c>
       <c r="F70" s="2"/>
@@ -2199,7 +2223,7 @@
       <c r="D71" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E71" s="30" t="s">
+      <c r="E71" s="13" t="s">
         <v>93</v>
       </c>
       <c r="F71" s="2"/>
@@ -2217,7 +2241,7 @@
       <c r="D72" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E72" s="29" t="s">
+      <c r="E72" s="13" t="s">
         <v>94</v>
       </c>
       <c r="F72" s="2"/>
@@ -2235,7 +2259,7 @@
       <c r="D73" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E73" s="29" t="s">
+      <c r="E73" s="13" t="s">
         <v>95</v>
       </c>
       <c r="F73" s="2"/>
@@ -2253,7 +2277,7 @@
       <c r="D74" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E74" s="29" t="s">
+      <c r="E74" s="13" t="s">
         <v>96</v>
       </c>
       <c r="F74" s="2"/>
@@ -2271,7 +2295,7 @@
       <c r="D75" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E75" s="29" t="s">
+      <c r="E75" s="13" t="s">
         <v>97</v>
       </c>
       <c r="F75" s="2"/>
@@ -2289,7 +2313,7 @@
       <c r="D76" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E76" s="30" t="s">
+      <c r="E76" s="13" t="s">
         <v>98</v>
       </c>
       <c r="F76" s="2"/>
@@ -2307,7 +2331,7 @@
       <c r="D77" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E77" s="30" t="s">
+      <c r="E77" s="13" t="s">
         <v>99</v>
       </c>
       <c r="F77" s="2"/>
@@ -2325,7 +2349,7 @@
       <c r="D78" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E78" s="30" t="s">
+      <c r="E78" s="13" t="s">
         <v>100</v>
       </c>
       <c r="F78" s="2"/>
@@ -2359,104 +2383,219 @@
       <c r="F81" s="31"/>
     </row>
     <row r="82" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C82" s="10"/>
-      <c r="E82" s="12"/>
-    </row>
-    <row r="83" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="7"/>
-      <c r="B83" s="21"/>
-      <c r="C83" s="11"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="2"/>
+      <c r="A82" s="4">
+        <v>43613</v>
+      </c>
+      <c r="B82" s="20">
+        <v>7</v>
+      </c>
+      <c r="C82" s="10">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E82" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>43613</v>
+      </c>
+      <c r="B83" s="20">
+        <v>7</v>
+      </c>
+      <c r="C83" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E83" s="12" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="84" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="4">
+        <v>43613</v>
+      </c>
+      <c r="B84" s="20">
+        <v>7</v>
+      </c>
+      <c r="C84" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E84" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>43613</v>
+      </c>
+      <c r="B85" s="20">
+        <v>7</v>
+      </c>
+      <c r="C85" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E85" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>43613</v>
+      </c>
+      <c r="B86" s="20">
+        <v>7</v>
+      </c>
+      <c r="C86" s="10">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E86" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
+        <v>43614</v>
+      </c>
+      <c r="B87" s="20">
+        <v>7</v>
+      </c>
+      <c r="C87" s="10">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E87" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <v>43614</v>
+      </c>
+      <c r="B88" s="20">
+        <v>7</v>
+      </c>
+      <c r="C88" s="10">
+        <v>9.375E-2</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E88" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="7"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="2"/>
+    </row>
+    <row r="90" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C84" s="10">
-        <f>SUM(C82:C82)</f>
+      <c r="C90" s="10">
+        <f>SUM(C82:C89)</f>
+        <v>0.4375</v>
+      </c>
+      <c r="E90" s="12"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B91" s="31"/>
+      <c r="C91" s="31"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="31"/>
+      <c r="F91" s="31"/>
+    </row>
+    <row r="92" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C92" s="10"/>
+      <c r="E92" s="12"/>
+    </row>
+    <row r="93" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="7"/>
+      <c r="B93" s="21"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C94" s="10">
+        <f>SUM(C92:C92)</f>
         <v>0</v>
       </c>
-      <c r="E84" s="12"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="B85" s="31"/>
-      <c r="C85" s="31"/>
-      <c r="D85" s="31"/>
-      <c r="E85" s="31"/>
-      <c r="F85" s="31"/>
-    </row>
-    <row r="86" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C86" s="10"/>
-      <c r="E86" s="12"/>
-    </row>
-    <row r="87" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="7"/>
-      <c r="B87" s="21"/>
-      <c r="C87" s="11"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="2"/>
-    </row>
-    <row r="88" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C88" s="10">
-        <f>SUM(C86:C86)</f>
-        <v>0</v>
-      </c>
-      <c r="E88" s="12"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="6"/>
-      <c r="F89" s="6"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="6"/>
-      <c r="F90" s="6"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="6"/>
-      <c r="F91" s="6"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="6"/>
-      <c r="F92" s="6"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="6"/>
-      <c r="F93" s="6"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="6"/>
-      <c r="F94" s="6"/>
+      <c r="E94" s="12"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="5"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="5"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="5"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="5"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="5"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A85:F85"/>
+    <mergeCell ref="A91:F91"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A35:F35"/>
@@ -2464,6 +2603,6 @@
     <mergeCell ref="A81:F81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="92" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="89" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update all documentation and correction of many small bugs
</commit_message>
<xml_diff>
--- a/Documentation/FBN_TPI_simulateur_trafic_routier_journal_travail.xlsx
+++ b/Documentation/FBN_TPI_simulateur_trafic_routier_journal_travail.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="116">
   <si>
     <t>Date</t>
   </si>
@@ -335,6 +335,51 @@
   </si>
   <si>
     <t>Mise en place de l'ecriture des résultats pour les priorités de droite</t>
+  </si>
+  <si>
+    <t>Suite et fin de l'écriture des résultats pour les priorités de droite</t>
+  </si>
+  <si>
+    <t>Suite de la création de la fonction de la simulation - partie feux vert / rouge</t>
+  </si>
+  <si>
+    <t>Implémentation des rêgles de conduites pour les feux (rouge / vert)</t>
+  </si>
+  <si>
+    <t>Suite de la création de la fonction de la simulation - giratoire</t>
+  </si>
+  <si>
+    <t>Implémentation des rêgles de conduites pour les giratoires</t>
+  </si>
+  <si>
+    <t>Suite et fin de l'implémentation des rêgles de conduite pour les giratoires</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Tests du resultat de la simulation</t>
+  </si>
+  <si>
+    <t>Ecriture du ducument d'installation</t>
+  </si>
+  <si>
+    <t>Ecriture du ducument d'utilisation</t>
+  </si>
+  <si>
+    <t>Ecriture de la conslusion du rapport</t>
+  </si>
+  <si>
+    <t>Définition du glossaire</t>
+  </si>
+  <si>
+    <t>Mise en place du document de résumé</t>
+  </si>
+  <si>
+    <t>Mise en page des documents et corrections</t>
+  </si>
+  <si>
+    <t>Préparation des rendus</t>
   </si>
 </sst>
 </file>
@@ -515,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -612,6 +657,27 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -896,7 +962,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,8 +1003,8 @@
         <v>6</v>
       </c>
       <c r="B4" s="25">
-        <f>Journal!C84</f>
-        <v>0</v>
+        <f>Journal!C90</f>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="21" x14ac:dyDescent="0.25">
@@ -946,8 +1012,8 @@
         <v>7</v>
       </c>
       <c r="B5" s="26">
-        <f>Journal!C88</f>
-        <v>0</v>
+        <f>Journal!C101</f>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.25">
@@ -956,7 +1022,7 @@
       </c>
       <c r="B6" s="27">
         <f>SUM(B1:B5)</f>
-        <v>2.8125</v>
+        <v>3.6875</v>
       </c>
     </row>
   </sheetData>
@@ -970,11 +1036,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E79" sqref="E79"/>
+      <pane ySplit="2" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2096,7 +2162,7 @@
       </c>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" s="8" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>43607</v>
       </c>
@@ -2109,12 +2175,12 @@
       <c r="D66" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E66" s="29" t="s">
+      <c r="E66" s="13" t="s">
         <v>88</v>
       </c>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" s="8" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>43607</v>
       </c>
@@ -2127,7 +2193,7 @@
       <c r="D67" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E67" s="29" t="s">
+      <c r="E67" s="13" t="s">
         <v>89</v>
       </c>
       <c r="F67" s="2"/>
@@ -2145,7 +2211,7 @@
       <c r="D68" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E68" s="30" t="s">
+      <c r="E68" s="13" t="s">
         <v>90</v>
       </c>
       <c r="F68" s="2"/>
@@ -2163,7 +2229,7 @@
       <c r="D69" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E69" s="30" t="s">
+      <c r="E69" s="13" t="s">
         <v>91</v>
       </c>
       <c r="F69" s="2"/>
@@ -2181,7 +2247,7 @@
       <c r="D70" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E70" s="30" t="s">
+      <c r="E70" s="13" t="s">
         <v>92</v>
       </c>
       <c r="F70" s="2"/>
@@ -2199,7 +2265,7 @@
       <c r="D71" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E71" s="30" t="s">
+      <c r="E71" s="13" t="s">
         <v>93</v>
       </c>
       <c r="F71" s="2"/>
@@ -2217,7 +2283,7 @@
       <c r="D72" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E72" s="29" t="s">
+      <c r="E72" s="13" t="s">
         <v>94</v>
       </c>
       <c r="F72" s="2"/>
@@ -2235,7 +2301,7 @@
       <c r="D73" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E73" s="29" t="s">
+      <c r="E73" s="13" t="s">
         <v>95</v>
       </c>
       <c r="F73" s="2"/>
@@ -2253,7 +2319,7 @@
       <c r="D74" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E74" s="29" t="s">
+      <c r="E74" s="13" t="s">
         <v>96</v>
       </c>
       <c r="F74" s="2"/>
@@ -2271,7 +2337,7 @@
       <c r="D75" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E75" s="29" t="s">
+      <c r="E75" s="13" t="s">
         <v>97</v>
       </c>
       <c r="F75" s="2"/>
@@ -2289,7 +2355,7 @@
       <c r="D76" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E76" s="30" t="s">
+      <c r="E76" s="13" t="s">
         <v>98</v>
       </c>
       <c r="F76" s="2"/>
@@ -2307,7 +2373,7 @@
       <c r="D77" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E77" s="30" t="s">
+      <c r="E77" s="13" t="s">
         <v>99</v>
       </c>
       <c r="F77" s="2"/>
@@ -2325,7 +2391,7 @@
       <c r="D78" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E78" s="30" t="s">
+      <c r="E78" s="13" t="s">
         <v>100</v>
       </c>
       <c r="F78" s="2"/>
@@ -2359,104 +2425,353 @@
       <c r="F81" s="31"/>
     </row>
     <row r="82" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C82" s="10"/>
-      <c r="E82" s="12"/>
-    </row>
-    <row r="83" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="7"/>
-      <c r="B83" s="21"/>
-      <c r="C83" s="11"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="2"/>
+      <c r="A82" s="4">
+        <v>43613</v>
+      </c>
+      <c r="B82" s="20">
+        <v>7</v>
+      </c>
+      <c r="C82" s="10">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E82" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>43613</v>
+      </c>
+      <c r="B83" s="20">
+        <v>7</v>
+      </c>
+      <c r="C83" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E83" s="12" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="84" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="4">
+        <v>43613</v>
+      </c>
+      <c r="B84" s="20">
+        <v>7</v>
+      </c>
+      <c r="C84" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E84" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>43613</v>
+      </c>
+      <c r="B85" s="20">
+        <v>7</v>
+      </c>
+      <c r="C85" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E85" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>43613</v>
+      </c>
+      <c r="B86" s="20">
+        <v>7</v>
+      </c>
+      <c r="C86" s="10">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E86" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
+        <v>43614</v>
+      </c>
+      <c r="B87" s="20">
+        <v>7</v>
+      </c>
+      <c r="C87" s="10">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E87" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <v>43614</v>
+      </c>
+      <c r="B88" s="20">
+        <v>7</v>
+      </c>
+      <c r="C88" s="10">
+        <v>9.375E-2</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E88" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="7"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="2"/>
+    </row>
+    <row r="90" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C84" s="10">
-        <f>SUM(C82:C82)</f>
-        <v>0</v>
-      </c>
-      <c r="E84" s="12"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="31" t="s">
+      <c r="C90" s="10">
+        <f>SUM(C82:C89)</f>
+        <v>0.4375</v>
+      </c>
+      <c r="E90" s="12"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B85" s="31"/>
-      <c r="C85" s="31"/>
-      <c r="D85" s="31"/>
-      <c r="E85" s="31"/>
-      <c r="F85" s="31"/>
-    </row>
-    <row r="86" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C86" s="10"/>
-      <c r="E86" s="12"/>
-    </row>
-    <row r="87" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="7"/>
-      <c r="B87" s="21"/>
-      <c r="C87" s="11"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="2"/>
-    </row>
-    <row r="88" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
+      <c r="B91" s="31"/>
+      <c r="C91" s="31"/>
+      <c r="D91" s="31"/>
+      <c r="E91" s="31"/>
+      <c r="F91" s="31"/>
+    </row>
+    <row r="92" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>43589</v>
+      </c>
+      <c r="B92" s="20">
+        <v>8</v>
+      </c>
+      <c r="C92" s="10">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E92" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>43589</v>
+      </c>
+      <c r="B93" s="20">
+        <v>8</v>
+      </c>
+      <c r="C93" s="10">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E93" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>43589</v>
+      </c>
+      <c r="B94" s="20">
+        <v>8</v>
+      </c>
+      <c r="C94" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E94" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4">
+        <v>43589</v>
+      </c>
+      <c r="B95" s="20">
+        <v>8</v>
+      </c>
+      <c r="C95" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E95" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>43589</v>
+      </c>
+      <c r="B96" s="20">
+        <v>8</v>
+      </c>
+      <c r="C96" s="10">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E96" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>43589</v>
+      </c>
+      <c r="B97" s="20">
+        <v>8</v>
+      </c>
+      <c r="C97" s="10">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E97" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" s="8" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="7">
+        <v>43589</v>
+      </c>
+      <c r="B98" s="21">
+        <v>8</v>
+      </c>
+      <c r="C98" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E98" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:6" s="39" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="33">
+        <v>43590</v>
+      </c>
+      <c r="B99" s="34">
+        <v>8</v>
+      </c>
+      <c r="C99" s="35">
+        <v>0.15625</v>
+      </c>
+      <c r="D99" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E99" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F99" s="38"/>
+    </row>
+    <row r="100" spans="1:6" s="39" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="33"/>
+      <c r="B100" s="34"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="36"/>
+      <c r="E100" s="37"/>
+      <c r="F100" s="38"/>
+    </row>
+    <row r="101" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C88" s="10">
-        <f>SUM(C86:C86)</f>
-        <v>0</v>
-      </c>
-      <c r="E88" s="12"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="6"/>
-      <c r="F89" s="6"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="6"/>
-      <c r="F90" s="6"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="6"/>
-      <c r="F91" s="6"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="6"/>
-      <c r="F92" s="6"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="6"/>
-      <c r="F93" s="6"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="6"/>
-      <c r="F94" s="6"/>
+      <c r="C101" s="10">
+        <f>SUM(C92:C100)</f>
+        <v>0.4375</v>
+      </c>
+      <c r="E101" s="12"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="5"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="5"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="5"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="5"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="5"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="6"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="5"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A85:F85"/>
+    <mergeCell ref="A91:F91"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A35:F35"/>
@@ -2464,6 +2779,6 @@
     <mergeCell ref="A81:F81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="92" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="89" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>